<commit_message>
[qos] complete the study of chip manual about qos [math] continuous learning [english] words and reading
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-01.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +115,14 @@
   </si>
   <si>
     <t>看数学视频，泰勒级数那一节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -375,7 +383,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -449,6 +457,93 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -464,6 +559,9 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -479,95 +577,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="58" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -843,7 +854,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -854,7 +865,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H9" sqref="H9:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -869,22 +880,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="72"/>
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
@@ -905,7 +916,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="67" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="30" t="s">
@@ -918,13 +929,17 @@
         <v>10</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="38"/>
+      <c r="H3" s="68">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="36"/>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="65"/>
+      <c r="B4" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -934,41 +949,51 @@
         <v>16</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="39"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="73">
+        <v>43161</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="39"/>
+      <c r="H5" s="69"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="73">
+        <v>43162</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="39"/>
+      <c r="H6" s="69"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
@@ -976,12 +1001,14 @@
         <v>9</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="40"/>
+      <c r="H7" s="70"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="36"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="30" t="s">
         <v>8</v>
       </c>
@@ -990,93 +1017,97 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G8" s="29"/>
-      <c r="H8" s="31"/>
+      <c r="H8" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="51"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="61"/>
-      <c r="B10" s="60"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="52"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="61"/>
-      <c r="B11" s="54"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="61"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="50"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="61"/>
-      <c r="B13" s="55"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="52"/>
+      <c r="H13" s="50"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="61"/>
-      <c r="B14" s="56"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="53"/>
+      <c r="H14" s="51"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="61"/>
-      <c r="B15" s="54"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="51"/>
+      <c r="H15" s="49"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="61"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="56"/>
+      <c r="H16" s="54"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="61"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1085,8 +1116,8 @@
       <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="60"/>
-      <c r="B18" s="56"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1095,194 +1126,194 @@
       <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="47"/>
-      <c r="B19" s="47"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="12"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="67"/>
+      <c r="H19" s="44"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="49"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="18"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="68"/>
+      <c r="H20" s="45"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="49"/>
-      <c r="B21" s="49"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="18"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="68"/>
+      <c r="H21" s="45"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="48"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="69"/>
+      <c r="H22" s="46"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="70"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="22"/>
       <c r="C23" s="17"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="65"/>
+      <c r="H23" s="42"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="71"/>
-      <c r="B24" s="58"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="59"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="66"/>
+      <c r="H24" s="43"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="71"/>
-      <c r="B25" s="58"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="1"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="66"/>
+      <c r="H25" s="43"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="71"/>
-      <c r="B26" s="43"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="1"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="66"/>
+      <c r="H26" s="43"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="71"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="15"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="66"/>
+      <c r="H27" s="43"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="47"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="24"/>
       <c r="C28" s="23"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
-      <c r="H28" s="62"/>
+      <c r="H28" s="39"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="49"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="24"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="63"/>
+      <c r="H29" s="40"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="49"/>
-      <c r="B30" s="47"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="63"/>
+      <c r="H30" s="40"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="64"/>
+      <c r="H31" s="41"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="43"/>
-      <c r="B32" s="43"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="57"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
-      <c r="H32" s="57"/>
+      <c r="H32" s="55"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="60"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="19"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="46"/>
+      <c r="H33" s="56"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="44"/>
-      <c r="B34" s="50"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="58"/>
       <c r="C34" s="19"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="46"/>
+      <c r="H34" s="56"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="44"/>
-      <c r="B35" s="45"/>
+      <c r="A35" s="60"/>
+      <c r="B35" s="61"/>
       <c r="C35" s="19"/>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
-      <c r="H35" s="46"/>
+      <c r="H35" s="56"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="44"/>
-      <c r="B36" s="46"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="56"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
-      <c r="H36" s="46"/>
+      <c r="H36" s="56"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="44"/>
-      <c r="B37" s="46"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
-      <c r="H37" s="46"/>
+      <c r="H37" s="56"/>
     </row>
     <row r="38" spans="1:8" ht="14.25" customHeight="1">
       <c r="A38" s="27"/>
@@ -1296,6 +1327,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="H32:H37"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B15:B18"/>
     <mergeCell ref="A9:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="H28:H31"/>
@@ -1306,21 +1352,6 @@
     <mergeCell ref="H9:H14"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H32:H37"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>